<commit_message>
test/add acceptance test for case with stix
</commit_message>
<xml_diff>
--- a/tests/test_data/TestCase1_38-1_no_housing_stix/DV01A.xlsx
+++ b/tests/test_data/TestCase1_38-1_no_housing_stix/DV01A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VRM\Gegevens 38-1\tests\TestCase1_38-1_no_housing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hauth\bitbucket\Veiligheidsrendement\tests\test_data\TestCase1_38-1_no_housing_stix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305C3614-2A02-459D-B5AE-83DAF9A71F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEB71D1-FFE0-4635-9ED6-3EDF66A2914D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="108">
   <si>
     <t>Value</t>
   </si>
@@ -130,25 +130,10 @@
     <t>dSF</t>
   </si>
   <si>
-    <t>Grondversterking binnenwaarts 2045</t>
-  </si>
-  <si>
     <t>Soil reinforcement</t>
   </si>
   <si>
-    <t>combinable</t>
-  </si>
-  <si>
     <t>inward</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Grondversterking binnenwaarts 2025</t>
-  </si>
-  <si>
-    <t>Grondversterking met stabiliteitsscherm 2045</t>
   </si>
   <si>
     <t>full</t>
@@ -726,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -783,7 +768,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,9 +829,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -899,13 +886,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -914,25 +901,25 @@
         <v>37</v>
       </c>
       <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
         <v>38</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>30</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -940,19 +927,16 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -969,31 +953,31 @@
       <c r="K3">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
-        <v>39</v>
+      <c r="M3">
+        <v>1E-3</v>
+      </c>
+      <c r="N3">
+        <v>9.9999999999999998E-13</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>30</v>
@@ -1007,28 +991,28 @@
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4" t="s">
-        <v>43</v>
+      <c r="M4">
+        <v>1E-8</v>
+      </c>
+      <c r="N4">
+        <v>9.9999999999999998E-13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1045,118 +1029,7 @@
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="L5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>30</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>1E-3</v>
-      </c>
-      <c r="N6">
-        <v>9.9999999999999998E-13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="M7">
-        <v>1E-8</v>
-      </c>
-      <c r="N7">
-        <v>9.9999999999999998E-13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>30</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="O8">
+      <c r="O5">
         <v>0.2</v>
       </c>
     </row>
@@ -1175,15 +1048,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>-17</v>
@@ -1194,7 +1067,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1205,7 +1078,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>3.5</v>
@@ -1216,7 +1089,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>25</v>
@@ -1227,7 +1100,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>42</v>
@@ -1238,7 +1111,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>47</v>
@@ -1262,15 +1135,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1278,7 +1151,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1286,7 +1159,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1294,7 +1167,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1302,7 +1175,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1310,7 +1183,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1318,7 +1191,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1326,7 +1199,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1334,7 +1207,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1342,7 +1215,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1350,7 +1223,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1358,7 +1231,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1366,7 +1239,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1374,7 +1247,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1382,7 +1255,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1390,7 +1263,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1398,7 +1271,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1406,7 +1279,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1414,7 +1287,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1422,7 +1295,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1430,7 +1303,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1438,7 +1311,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1446,7 +1319,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1454,7 +1327,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1462,7 +1335,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1470,7 +1343,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1478,7 +1351,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1486,7 +1359,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1494,7 +1367,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1502,7 +1375,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1510,7 +1383,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1518,7 +1391,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1526,7 +1399,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1534,7 +1407,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1542,7 +1415,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1550,7 +1423,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1558,7 +1431,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1566,7 +1439,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1574,7 +1447,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1582,7 +1455,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1590,7 +1463,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1598,7 +1471,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1606,7 +1479,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1614,7 +1487,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1622,7 +1495,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1630,7 +1503,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1638,7 +1511,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1646,7 +1519,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1654,7 +1527,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1662,7 +1535,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B51">
         <v>0</v>

</xml_diff>